<commit_message>
enable case sensitivity check_docu_excel
</commit_message>
<xml_diff>
--- a/tests/testthat/helper_codebook_p3.xlsx
+++ b/tests/testthat/helper_codebook_p3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Packages\eatFDZ\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B22F0790-A16D-40A5-92E4-DF9BA84CB28F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259EF6AA-5A7E-4FD9-B7A8-57AA4BACED69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13425" xr2:uid="{D26A02C0-366E-42D4-8EE1-23B9CF1F09FA}"/>
   </bookViews>
@@ -39,10 +39,10 @@
     <t xml:space="preserve">ID-Variable </t>
   </si>
   <si>
-    <t xml:space="preserve">Var3 </t>
-  </si>
-  <si>
     <t>Variable 3, weitere Informationen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var3 </t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,10 +440,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>